<commit_message>
put some data to cell
</commit_message>
<xml_diff>
--- a/excel/test.xlsx
+++ b/excel/test.xlsx
@@ -1,54 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="4">
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>EUR</t>
-  </si>
-  <si>
-    <t>RUR</t>
-  </si>
-  <si>
-    <t>fgf</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -67,22 +46,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -348,161 +386,209 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:E23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="C3:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3">
+    <row r="3">
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4">
+    <row r="4">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5">
+    <row r="5">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>RUR</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
         <v>2222</v>
       </c>
     </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6">
+    <row r="6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7">
+    <row r="7">
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8">
+      <c r="G7" t="n">
+        <v>4019</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>RUR</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
         <v>54343</v>
       </c>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9">
+    <row r="9">
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10">
+    <row r="10">
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
         <v>566</v>
       </c>
     </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11">
+    <row r="11">
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>RUR</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
         <v>344343</v>
       </c>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1">
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15">
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E15" s="1" t="n">
         <v>555.5</v>
       </c>
     </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16">
+    <row r="16">
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
         <v>445</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17">
+    <row r="17">
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>RUR</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
         <v>5433534</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C18" t="s">
-        <v>0</v>
-      </c>
-      <c r="E18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19">
+    <row r="18">
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>fgf</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
         <v>3532</v>
       </c>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
-        <v>2</v>
-      </c>
-      <c r="E20">
+    <row r="20">
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>RUR</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
         <v>454543</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C21" t="s">
-        <v>0</v>
-      </c>
-      <c r="E21">
+    <row r="21">
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
         <v>554</v>
       </c>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22">
+    <row r="22">
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C23" t="s">
-        <v>2</v>
-      </c>
-      <c r="E23">
+    <row r="23">
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>RUR</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
         <v>45354</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="90" verticalDpi="90"/>
 </worksheet>
 </file>
</xml_diff>